<commit_message>
Assignment 2 is completed
</commit_message>
<xml_diff>
--- a/src/test/resources/externalTestData/QA_WalletHub_TestData.xlsx
+++ b/src/test/resources/externalTestData/QA_WalletHub_TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Wallethub\WalletHubSeleniumFramework\src\test\resources\externalTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD588666-7A82-44EC-BEC2-33286F19BADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E12008F-7BA7-4304-AF2E-5255555A202C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="39">
   <si>
     <t>Portal</t>
   </si>
@@ -135,6 +135,15 @@
   </si>
   <si>
     <t>Yes[AutoGenerate]</t>
+  </si>
+  <si>
+    <t>Message Length</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>200</t>
   </si>
 </sst>
 </file>
@@ -194,7 +203,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -208,6 +217,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -701,10 +713,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58065CC2-CB6D-4A8F-8338-35814EB4F34F}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -720,9 +732,10 @@
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.36328125" style="3" customWidth="1"/>
     <col min="11" max="11" width="37.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -756,8 +769,11 @@
       <c r="K1" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="L1" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
@@ -785,11 +801,14 @@
       <c r="I2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="2">
-        <v>4</v>
+      <c r="J2" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>35</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -800,5 +819,8 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
+  <ignoredErrors>
+    <ignoredError sqref="J2 L2" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>